<commit_message>
Incl France and NL
</commit_message>
<xml_diff>
--- a/data/WHO.xlsx
+++ b/data/WHO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data2\github\who-data\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data2\github\Corona-Virus-WHO-Data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C1C29-3E28-4B0C-A3FC-517FEDD01B0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A322C63E-16B9-441A-84F1-53E38B339859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48961237-978F-4759-94F6-8FF0FDD558F7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
   <si>
     <t>Country</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>France</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A32934-90FD-4A0C-A21C-93B5C66ACB46}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,119 +451,119 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>43897</v>
+        <v>43894</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>4636</v>
+        <v>2502</v>
       </c>
       <c r="D2">
-        <v>778</v>
+        <v>466</v>
       </c>
       <c r="E2">
-        <v>197</v>
+        <v>80</v>
       </c>
       <c r="F2">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>43897</v>
+        <v>43894</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>167</v>
+        <v>51</v>
       </c>
       <c r="D3">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>43898</v>
+        <v>43894</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>5883</v>
+        <v>28</v>
       </c>
       <c r="D4">
-        <v>1247</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>43898</v>
+        <v>43895</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>210</v>
+        <v>3089</v>
       </c>
       <c r="D5">
-        <v>43</v>
+        <v>587</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>43899</v>
+        <v>43895</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>7375</v>
+        <v>89</v>
       </c>
       <c r="D6">
-        <v>1492</v>
+        <v>38</v>
       </c>
       <c r="E6">
-        <v>366</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>43899</v>
+        <v>43895</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>277</v>
+        <v>38</v>
       </c>
       <c r="D7">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -565,42 +571,42 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>43900</v>
+        <v>43895</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>9172</v>
+        <v>282</v>
       </c>
       <c r="D8">
-        <v>1797</v>
+        <v>73</v>
       </c>
       <c r="E8">
-        <v>463</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>43900</v>
+        <v>43896</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>323</v>
+        <v>3858</v>
       </c>
       <c r="D9">
-        <v>46</v>
+        <v>769</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -608,125 +614,406 @@
         <v>43896</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>3858</v>
+        <v>118</v>
       </c>
       <c r="D10">
-        <v>769</v>
+        <v>29</v>
       </c>
       <c r="E10">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>43895</v>
+        <v>43896</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>3089</v>
+        <v>82</v>
       </c>
       <c r="D11">
-        <v>587</v>
+        <v>44</v>
       </c>
       <c r="E11">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>43894</v>
+        <v>43896</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>2502</v>
+        <v>420</v>
       </c>
       <c r="D12">
-        <v>466</v>
+        <v>138</v>
       </c>
       <c r="E12">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>43896</v>
+        <v>43897</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>118</v>
+        <v>4636</v>
       </c>
       <c r="D13">
-        <v>29</v>
+        <v>778</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>43895</v>
+        <v>43897</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14">
-        <v>89</v>
+        <v>167</v>
       </c>
       <c r="D14">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
+        <v>43897</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>128</v>
+      </c>
+      <c r="D15">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>43897</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>613</v>
+      </c>
+      <c r="D16">
+        <v>193</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>5883</v>
+      </c>
+      <c r="D17">
+        <v>1247</v>
+      </c>
+      <c r="E17">
+        <v>234</v>
+      </c>
+      <c r="F17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>210</v>
+      </c>
+      <c r="D18">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>188</v>
+      </c>
+      <c r="D19">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>706</v>
+      </c>
+      <c r="D20">
+        <v>93</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>7375</v>
+      </c>
+      <c r="D21">
+        <v>1492</v>
+      </c>
+      <c r="E21">
+        <v>366</v>
+      </c>
+      <c r="F21">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>277</v>
+      </c>
+      <c r="D22">
+        <v>67</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>265</v>
+      </c>
+      <c r="D23">
+        <v>77</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>1116</v>
+      </c>
+      <c r="D24">
+        <v>410</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>9172</v>
+      </c>
+      <c r="D25">
+        <v>1797</v>
+      </c>
+      <c r="E25">
+        <v>463</v>
+      </c>
+      <c r="F25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>323</v>
+      </c>
+      <c r="D26">
+        <v>46</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>321</v>
+      </c>
+      <c r="D27">
+        <v>56</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>1402</v>
+      </c>
+      <c r="D28">
+        <v>286</v>
+      </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
         <v>43894</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>51</v>
-      </c>
-      <c r="D15">
-        <v>12</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>212</v>
+      </c>
+      <c r="D29">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>